<commit_message>
Added some more results files, updated script for evaluation based on sentiment_analysis
</commit_message>
<xml_diff>
--- a/datasets_info/fidelity_experiments/fidelity_yelp.xlsx
+++ b/datasets_info/fidelity_experiments/fidelity_yelp.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mentos\Documents\Studia\Semestr 10\Magisterka\peter\PETER\datasets_info\fidelity_experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6AF844-99F9-4F12-9A0B-FB4D58929A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FBE844-B178-49D4-AEBD-0A0662AAD52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="420" windowWidth="24240" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13515" yWindow="1380" windowWidth="12735" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="2nd_eval" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
   <si>
     <t>GT dobre</t>
   </si>
@@ -160,6 +161,27 @@
   <si>
     <t>Podwójny rekomender</t>
   </si>
+  <si>
+    <t>Yelp</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>1st eval</t>
+  </si>
+  <si>
+    <t>Korelacja:</t>
+  </si>
+  <si>
+    <t>Ręczna predykcja oceny</t>
+  </si>
+  <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t>Korelacja</t>
+  </si>
 </sst>
 </file>
 
@@ -203,13 +225,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -495,9 +520,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R33" sqref="R33"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,11 +560,11 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
     </row>
     <row r="2" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G2" s="2"/>
@@ -4169,4 +4194,2190 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E47D7DA-951D-4AA0-9523-6B12D149129F}">
+  <dimension ref="B1:R102"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>3925</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="E3">
+        <v>0.5</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="Q3">
+        <f>ABS(M3-N3)</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f>SUM(Q3:Q102)</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>4693</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <v>5</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q67" si="0">ABS(M4-N4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>7149</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>9078</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>11035</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>5</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>12562</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
+      </c>
+      <c r="N8">
+        <v>4</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>14346</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
+      <c r="N9">
+        <v>5</v>
+      </c>
+      <c r="P9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>34326</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="E10">
+        <v>0.5</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <f>PEARSON(M3:M102,N3:N102)</f>
+        <v>0.54989410181768772</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>34981</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>5</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>37277</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>5</v>
+      </c>
+      <c r="N12">
+        <v>5</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>39921</v>
+      </c>
+      <c r="C13">
+        <v>0.5</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>4</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>44606</v>
+      </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="N14">
+        <v>4</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>44658</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>4</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>46009</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>48642</v>
+      </c>
+      <c r="C17">
+        <v>0.5</v>
+      </c>
+      <c r="E17">
+        <v>0.5</v>
+      </c>
+      <c r="M17">
+        <v>3</v>
+      </c>
+      <c r="N17">
+        <v>4</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>69129</v>
+      </c>
+      <c r="C18">
+        <v>0.5</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>4</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>82865</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>5</v>
+      </c>
+      <c r="N19">
+        <v>5</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>91174</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>5</v>
+      </c>
+      <c r="N20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>97331</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>5</v>
+      </c>
+      <c r="N21">
+        <v>4</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>114029</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+      <c r="N22">
+        <v>3</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>117077</v>
+      </c>
+      <c r="C23">
+        <v>0.5</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>5</v>
+      </c>
+      <c r="N23">
+        <v>4</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>119503</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>4</v>
+      </c>
+      <c r="N24">
+        <v>4</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>121053</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>5</v>
+      </c>
+      <c r="N25">
+        <v>5</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>124225</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>4</v>
+      </c>
+      <c r="N26">
+        <v>4</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>124777</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>2</v>
+      </c>
+      <c r="N27">
+        <v>3</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>125803</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>5</v>
+      </c>
+      <c r="N28">
+        <v>4</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>127114</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>5</v>
+      </c>
+      <c r="N29">
+        <v>5</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>128113</v>
+      </c>
+      <c r="C30">
+        <v>0.5</v>
+      </c>
+      <c r="E30">
+        <v>0.5</v>
+      </c>
+      <c r="M30">
+        <v>3</v>
+      </c>
+      <c r="N30">
+        <v>4</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>133939</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>5</v>
+      </c>
+      <c r="N31">
+        <v>5</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>136942</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>4</v>
+      </c>
+      <c r="N32">
+        <v>4</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>149245</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>5</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>153041</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>155530</v>
+      </c>
+      <c r="C35">
+        <v>0.5</v>
+      </c>
+      <c r="E35">
+        <v>0.5</v>
+      </c>
+      <c r="M35">
+        <v>2</v>
+      </c>
+      <c r="N35">
+        <v>4</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>157689</v>
+      </c>
+      <c r="C36">
+        <v>0.5</v>
+      </c>
+      <c r="E36">
+        <v>0.5</v>
+      </c>
+      <c r="M36">
+        <v>3</v>
+      </c>
+      <c r="N36">
+        <v>4</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>158262</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>2</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>163897</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>5</v>
+      </c>
+      <c r="N38">
+        <v>4</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>178349</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>5</v>
+      </c>
+      <c r="N39">
+        <v>5</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>181025</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0.5</v>
+      </c>
+      <c r="M40">
+        <v>4</v>
+      </c>
+      <c r="N40">
+        <v>4</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>181745</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>5</v>
+      </c>
+      <c r="N41">
+        <v>4</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>184153</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>5</v>
+      </c>
+      <c r="N42">
+        <v>4</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>185062</v>
+      </c>
+      <c r="C43">
+        <v>0.5</v>
+      </c>
+      <c r="E43">
+        <v>0.5</v>
+      </c>
+      <c r="M43">
+        <v>3</v>
+      </c>
+      <c r="N43">
+        <v>5</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>188695</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <v>4</v>
+      </c>
+      <c r="N44">
+        <v>4</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>189814</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>2</v>
+      </c>
+      <c r="N45">
+        <v>4</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>199450</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="M46">
+        <v>2</v>
+      </c>
+      <c r="N46">
+        <v>2</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>201367</v>
+      </c>
+      <c r="C47">
+        <v>0.5</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="M47">
+        <v>3</v>
+      </c>
+      <c r="N47">
+        <v>2</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>204070</v>
+      </c>
+      <c r="C48">
+        <v>0.5</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>5</v>
+      </c>
+      <c r="N48">
+        <v>3</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>206341</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>5</v>
+      </c>
+      <c r="N49">
+        <v>3</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>209345</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <v>5</v>
+      </c>
+      <c r="N50">
+        <v>4</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>214221</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="M51">
+        <v>5</v>
+      </c>
+      <c r="N51">
+        <v>4</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>218153</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="M52">
+        <v>3</v>
+      </c>
+      <c r="N52">
+        <v>3</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>220513</v>
+      </c>
+      <c r="C53">
+        <v>0.5</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="M53">
+        <v>3</v>
+      </c>
+      <c r="N53">
+        <v>3</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>224401</v>
+      </c>
+      <c r="C54">
+        <v>0.5</v>
+      </c>
+      <c r="E54">
+        <v>0.5</v>
+      </c>
+      <c r="M54">
+        <v>4</v>
+      </c>
+      <c r="N54">
+        <v>3</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>232221</v>
+      </c>
+      <c r="C55">
+        <v>0.5</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="M55">
+        <v>4</v>
+      </c>
+      <c r="N55">
+        <v>4</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>245097</v>
+      </c>
+      <c r="C56">
+        <v>0.5</v>
+      </c>
+      <c r="E56">
+        <v>0.5</v>
+      </c>
+      <c r="M56">
+        <v>3</v>
+      </c>
+      <c r="N56">
+        <v>3</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>249433</v>
+      </c>
+      <c r="C57">
+        <v>0.5</v>
+      </c>
+      <c r="E57">
+        <v>0.5</v>
+      </c>
+      <c r="M57">
+        <v>3</v>
+      </c>
+      <c r="N57">
+        <v>2</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>250187</v>
+      </c>
+      <c r="C58">
+        <v>0.5</v>
+      </c>
+      <c r="E58">
+        <v>0.5</v>
+      </c>
+      <c r="M58">
+        <v>3</v>
+      </c>
+      <c r="N58">
+        <v>4</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>253623</v>
+      </c>
+      <c r="C59">
+        <v>0.5</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>4</v>
+      </c>
+      <c r="N59">
+        <v>3</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>262353</v>
+      </c>
+      <c r="C60">
+        <v>0.5</v>
+      </c>
+      <c r="E60">
+        <v>0.5</v>
+      </c>
+      <c r="M60">
+        <v>3</v>
+      </c>
+      <c r="N60">
+        <v>4</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>263265</v>
+      </c>
+      <c r="C61">
+        <v>0.5</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="M61">
+        <v>3</v>
+      </c>
+      <c r="N61">
+        <v>4</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>272563</v>
+      </c>
+      <c r="C62">
+        <v>0.5</v>
+      </c>
+      <c r="E62">
+        <v>0.5</v>
+      </c>
+      <c r="M62">
+        <v>2</v>
+      </c>
+      <c r="N62">
+        <v>4</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>277686</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="M63">
+        <v>5</v>
+      </c>
+      <c r="N63">
+        <v>5</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>284121</v>
+      </c>
+      <c r="C64">
+        <v>0.5</v>
+      </c>
+      <c r="E64">
+        <v>0.5</v>
+      </c>
+      <c r="M64">
+        <v>5</v>
+      </c>
+      <c r="N64">
+        <v>3</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>296174</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="M65">
+        <v>4</v>
+      </c>
+      <c r="N65">
+        <v>3</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>296669</v>
+      </c>
+      <c r="C66">
+        <v>0.5</v>
+      </c>
+      <c r="E66">
+        <v>0.5</v>
+      </c>
+      <c r="M66">
+        <v>3</v>
+      </c>
+      <c r="N66">
+        <v>3</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>296686</v>
+      </c>
+      <c r="C67">
+        <v>0.5</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="M67">
+        <v>4</v>
+      </c>
+      <c r="N67">
+        <v>3</v>
+      </c>
+      <c r="Q67">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>305259</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="M68">
+        <v>2</v>
+      </c>
+      <c r="N68">
+        <v>3</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" ref="Q68:Q101" si="1">ABS(M68-N68)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>305929</v>
+      </c>
+      <c r="C69">
+        <v>0.5</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="M69">
+        <v>4</v>
+      </c>
+      <c r="N69">
+        <v>3</v>
+      </c>
+      <c r="Q69">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>314570</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="M70">
+        <v>5</v>
+      </c>
+      <c r="N70">
+        <v>5</v>
+      </c>
+      <c r="Q70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>335459</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="M71">
+        <v>2</v>
+      </c>
+      <c r="N71">
+        <v>2</v>
+      </c>
+      <c r="Q71">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>339765</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="M72">
+        <v>1</v>
+      </c>
+      <c r="N72">
+        <v>3</v>
+      </c>
+      <c r="Q72">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>343515</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="M73">
+        <v>5</v>
+      </c>
+      <c r="N73">
+        <v>5</v>
+      </c>
+      <c r="Q73">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>346353</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <v>3</v>
+      </c>
+      <c r="N74">
+        <v>4</v>
+      </c>
+      <c r="Q74">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>359643</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="M75">
+        <v>5</v>
+      </c>
+      <c r="N75">
+        <v>5</v>
+      </c>
+      <c r="Q75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>366238</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="M76">
+        <v>5</v>
+      </c>
+      <c r="N76">
+        <v>5</v>
+      </c>
+      <c r="Q76">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>369143</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>2</v>
+      </c>
+      <c r="N77">
+        <v>4</v>
+      </c>
+      <c r="Q77">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>375611</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="M78">
+        <v>4</v>
+      </c>
+      <c r="N78">
+        <v>4</v>
+      </c>
+      <c r="Q78">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>375915</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="M79">
+        <v>1</v>
+      </c>
+      <c r="N79">
+        <v>2</v>
+      </c>
+      <c r="Q79">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>379179</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="M80">
+        <v>5</v>
+      </c>
+      <c r="N80">
+        <v>5</v>
+      </c>
+      <c r="Q80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>380106</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="H81" t="s">
+        <v>43</v>
+      </c>
+      <c r="M81">
+        <v>5</v>
+      </c>
+      <c r="N81">
+        <v>4</v>
+      </c>
+      <c r="Q81">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>393315</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <f>COUNTIF(C$3:C$102,G82)</f>
+        <v>9</v>
+      </c>
+      <c r="M82">
+        <v>4</v>
+      </c>
+      <c r="N82">
+        <v>4</v>
+      </c>
+      <c r="Q82">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>398398</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="G83">
+        <v>0.5</v>
+      </c>
+      <c r="H83">
+        <f t="shared" ref="H83:H84" si="2">COUNTIF(C$3:C$102,G83)</f>
+        <v>36</v>
+      </c>
+      <c r="M83">
+        <v>4</v>
+      </c>
+      <c r="N83">
+        <v>5</v>
+      </c>
+      <c r="Q83">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>402610</v>
+      </c>
+      <c r="C84">
+        <v>0.5</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="M84">
+        <v>2</v>
+      </c>
+      <c r="N84">
+        <v>3</v>
+      </c>
+      <c r="Q84">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>407854</v>
+      </c>
+      <c r="C85">
+        <v>0.5</v>
+      </c>
+      <c r="E85">
+        <v>0.5</v>
+      </c>
+      <c r="M85">
+        <v>3</v>
+      </c>
+      <c r="N85">
+        <v>5</v>
+      </c>
+      <c r="Q85">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>411783</v>
+      </c>
+      <c r="C86">
+        <v>0.5</v>
+      </c>
+      <c r="E86">
+        <v>0.5</v>
+      </c>
+      <c r="H86" t="s">
+        <v>45</v>
+      </c>
+      <c r="M86">
+        <v>3</v>
+      </c>
+      <c r="N86">
+        <v>3</v>
+      </c>
+      <c r="Q86">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>415862</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <f>PEARSON(C3:C102,E3:E102)</f>
+        <v>0.77649570555671621</v>
+      </c>
+      <c r="M87">
+        <v>4</v>
+      </c>
+      <c r="N87">
+        <v>5</v>
+      </c>
+      <c r="Q87">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>418957</v>
+      </c>
+      <c r="C88">
+        <v>0.5</v>
+      </c>
+      <c r="E88">
+        <v>0.5</v>
+      </c>
+      <c r="M88">
+        <v>3</v>
+      </c>
+      <c r="N88">
+        <v>2</v>
+      </c>
+      <c r="Q88">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>422517</v>
+      </c>
+      <c r="C89">
+        <v>0.5</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="M89">
+        <v>3</v>
+      </c>
+      <c r="N89">
+        <v>5</v>
+      </c>
+      <c r="Q89">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>428837</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
+      <c r="M90">
+        <v>5</v>
+      </c>
+      <c r="N90">
+        <v>5</v>
+      </c>
+      <c r="Q90">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>431257</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="M91">
+        <v>5</v>
+      </c>
+      <c r="N91">
+        <v>5</v>
+      </c>
+      <c r="Q91">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>444805</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="M92">
+        <v>2</v>
+      </c>
+      <c r="N92">
+        <v>2</v>
+      </c>
+      <c r="Q92">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>447517</v>
+      </c>
+      <c r="C93">
+        <v>0.5</v>
+      </c>
+      <c r="E93">
+        <v>0.5</v>
+      </c>
+      <c r="M93">
+        <v>1</v>
+      </c>
+      <c r="N93">
+        <v>3</v>
+      </c>
+      <c r="Q93">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>454359</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="M94">
+        <v>5</v>
+      </c>
+      <c r="N94">
+        <v>5</v>
+      </c>
+      <c r="Q94">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>456226</v>
+      </c>
+      <c r="C95">
+        <v>0.5</v>
+      </c>
+      <c r="E95">
+        <v>0.5</v>
+      </c>
+      <c r="M95">
+        <v>3</v>
+      </c>
+      <c r="N95">
+        <v>4</v>
+      </c>
+      <c r="Q95">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>457893</v>
+      </c>
+      <c r="C96">
+        <v>0.5</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="M96">
+        <v>4</v>
+      </c>
+      <c r="N96">
+        <v>3</v>
+      </c>
+      <c r="Q96">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>459962</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="M97">
+        <v>5</v>
+      </c>
+      <c r="N97">
+        <v>4</v>
+      </c>
+      <c r="Q97">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>466393</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="M98">
+        <v>5</v>
+      </c>
+      <c r="N98">
+        <v>4</v>
+      </c>
+      <c r="Q98">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>466945</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="M99">
+        <v>2</v>
+      </c>
+      <c r="N99">
+        <v>2</v>
+      </c>
+      <c r="Q99">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>476899</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0.5</v>
+      </c>
+      <c r="M100">
+        <v>3</v>
+      </c>
+      <c r="N100">
+        <v>5</v>
+      </c>
+      <c r="Q100">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>501217</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="M101">
+        <v>1</v>
+      </c>
+      <c r="N101">
+        <v>2</v>
+      </c>
+      <c r="Q101">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>516165</v>
+      </c>
+      <c r="C102">
+        <v>0.5</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+      <c r="M102">
+        <v>1</v>
+      </c>
+      <c r="N102">
+        <v>3</v>
+      </c>
+      <c r="Q102">
+        <f>ABS(M102-N102)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>